<commit_message>
Dane_termometrow.xlsx - wprowadzono dane innej sondy, 1114 ma prawdopodobnie zle wyliczone wspólczynniki w świadectwie
</commit_message>
<xml_diff>
--- a/Dane_termometrow.xlsx
+++ b/Dane_termometrow.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="5685_1114" sheetId="1" r:id="rId1"/>
-    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="5699_1198" sheetId="4" r:id="rId2"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId3"/>
+    <sheet name="Arkusz3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Typ:</t>
   </si>
@@ -102,8 +103,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -194,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -228,6 +230,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -533,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -727,13 +732,203 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>5699</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1198</v>
+      </c>
+      <c r="C4" s="12">
+        <v>44554</v>
+      </c>
+      <c r="D4" s="8">
+        <v>25.618327000000001</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4.7999999999999998E-6</v>
+      </c>
+      <c r="F4" s="4">
+        <v>660.32299999999998</v>
+      </c>
+      <c r="G4" s="4">
+        <v>3.37546422</v>
+      </c>
+      <c r="H4" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="F5" s="4">
+        <v>419.52699999999999</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2.56858298</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.6999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="F6" s="4">
+        <v>231.928</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1.89261521</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="F7" s="4">
+        <v>-38.834400000000002</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.84416743999999999</v>
+      </c>
+      <c r="H7" s="13">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="F8" s="4">
+        <v>-189.3442</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.21599515</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -747,4 +942,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dane_termometrow.xlsx - dodano zakładkę ze sprawdzeniem poprawności świadectwa dla zakresu 0,01 - 660.323
</commit_message>
<xml_diff>
--- a/Dane_termometrow.xlsx
+++ b/Dane_termometrow.xlsx
@@ -4,20 +4,41 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="5685_1114" sheetId="1" r:id="rId1"/>
     <sheet name="5699_1198" sheetId="4" r:id="rId2"/>
-    <sheet name="Arkusz2" sheetId="2" r:id="rId3"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId4"/>
+    <sheet name="spr_1114" sheetId="5" r:id="rId3"/>
+    <sheet name="spr_1198" sheetId="2" r:id="rId4"/>
+    <sheet name="Arkusz3" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames>
+    <definedName name="a" localSheetId="2">spr_1114!$A$9</definedName>
+    <definedName name="a">spr_1198!$A$9</definedName>
+    <definedName name="b" localSheetId="2">spr_1114!$A$10</definedName>
+    <definedName name="b">spr_1198!$A$10</definedName>
+    <definedName name="cc" localSheetId="2">spr_1114!$A$11</definedName>
+    <definedName name="cc">spr_1198!$A$11</definedName>
+    <definedName name="wal" localSheetId="2">spr_1114!$A$19</definedName>
+    <definedName name="wal">spr_1198!$A$19</definedName>
+    <definedName name="wral" localSheetId="2">spr_1114!$A$14</definedName>
+    <definedName name="wral">spr_1198!$A$14</definedName>
+    <definedName name="wrsn" localSheetId="2">spr_1114!$A$16</definedName>
+    <definedName name="wrsn">spr_1198!$A$16</definedName>
+    <definedName name="wrzn" localSheetId="2">spr_1114!$A$15</definedName>
+    <definedName name="wrzn">spr_1198!$A$15</definedName>
+    <definedName name="wsn" localSheetId="2">spr_1114!$A$21</definedName>
+    <definedName name="wsn">spr_1198!$A$21</definedName>
+    <definedName name="wzn" localSheetId="2">spr_1114!$A$20</definedName>
+    <definedName name="wzn">spr_1198!$A$20</definedName>
+  </definedNames>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>Typ:</t>
   </si>
@@ -98,16 +119,113 @@
   <si>
     <t>Expire_date</t>
   </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Wr</t>
+  </si>
+  <si>
+    <t>fh20</t>
+  </si>
+  <si>
+    <t>fsn</t>
+  </si>
+  <si>
+    <t>fzn</t>
+  </si>
+  <si>
+    <t>fal</t>
+  </si>
+  <si>
+    <t>wr_calc</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>Wral</t>
+  </si>
+  <si>
+    <t>WrZn</t>
+  </si>
+  <si>
+    <t>WrSn</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>WfpAl</t>
+  </si>
+  <si>
+    <t>WfpZn</t>
+  </si>
+  <si>
+    <t>WfpSn</t>
+  </si>
+  <si>
+    <r>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>W_sw</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>W_calc</t>
+    </r>
+  </si>
+  <si>
+    <t>Sprawdzenie współczynników funkcji odchylenia ze świadectwa i wyliczonych zgodnie z MST-90. Jeżeli różnice są zgodne dla dowolnego w, to znaczy że dane są poprawnie wyliczone</t>
+  </si>
+  <si>
+    <t>Dane ze świadectwa</t>
+  </si>
+  <si>
+    <t>funkcje interpolujące</t>
+  </si>
+  <si>
+    <t>Dane z tablic MST-90</t>
+  </si>
+  <si>
+    <t>dane wyliczone (SciLab)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="172" formatCode="0.000000000"/>
+    <numFmt numFmtId="181" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="182" formatCode="0.00000000E+00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +246,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,8 +279,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -192,11 +341,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -234,6 +474,88 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -247,6 +569,346 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>557563</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Obraz 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7915275" y="438149"/>
+          <a:ext cx="8739538" cy="2238375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>169627</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Obraz 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8058150" y="2962275"/>
+          <a:ext cx="4551127" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>547571</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Obraz 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6896101" y="5857875"/>
+          <a:ext cx="7310320" cy="3629025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>557563</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Obraz 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6448425" y="438149"/>
+          <a:ext cx="8739538" cy="2238375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>20811</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Obraz 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6581776" y="2838450"/>
+          <a:ext cx="4381500" cy="3087861"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Obraz 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5676900" y="6457950"/>
+          <a:ext cx="7229475" cy="2876550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -538,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +1438,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -934,17 +1596,629 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="27">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E2" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="26">
+        <f>I5+I6*wrsn+I7*wrzn+I8*wral</f>
+        <v>2.5003491330545939</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E3" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="26">
+        <f>a*(F1-1)+b*(F1-1)^2+cc*(F1-1)^3</f>
+        <v>-3.5427221358749994E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E4" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="29">
+        <f>F1-F2</f>
+        <v>-3.4913305459394195E-4</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="19">
+        <f>((F1-wsn)*(F1-wzn)*(F1-wal))/((1-wsn)*(1-wzn)*(1-wal))</f>
+        <v>-1.0960197111552421E-2</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="22"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="19">
+        <f>((F1-1)*(F1-wzn)*(F1-wal))/((wsn-1)*(wsn-wzn)*(wsn-wal))</f>
+        <v>0.10061493983155403</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="19">
+        <f>((F1-1)*(F1-wsn)*(F1-wal))/((wzn-1)*(wzn-wsn)*(wzn-wal))</f>
+        <v>0.9323205591075574</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="19">
+        <f>((F1-1)*(F1-wsn)*(F1-wzn))/((wal-1)*(wal-wsn)*(wal-wzn))</f>
+        <v>-2.1975301827558993E-2</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>-2.6051786999999998E-4</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="48">
+        <v>-2.1371537544641301E-4</v>
+      </c>
+      <c r="E9" s="23"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>3.0380417000000001E-5</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="48">
+        <v>-1.43251789292556E-5</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>-9.4374361000000006E-6</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="49">
+        <v>1.0884977044838E-6</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="33"/>
+    </row>
+    <row r="14" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>3.3760086</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2.5689172999999998</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="46"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1.8927976799999999</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="47"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="33"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>3.3754346900000001</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>2.5685510300000001</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="38"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>1.89259628</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="39"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="41"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="41"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="41"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E24" s="39"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="41"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E25" s="42"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="E20:J25"/>
+    <mergeCell ref="C14:C16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="27">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E2" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="26">
+        <f>I5+I6*wrsn+I7*wrzn+I8*wral</f>
+        <v>2.5003180823822069</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E3" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="26">
+        <f>a*(F1-1)+b*(F1-1)^2+cc*(F1-1)^3</f>
+        <v>-3.1808484813750001E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E4" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="29">
+        <f>F1-F2</f>
+        <v>-3.1808238220687457E-4</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="19">
+        <f>((F1-wsn)*(F1-wzn)*(F1-wal))/((1-wsn)*(1-wzn)*(1-wal))</f>
+        <v>-1.0964741329934571E-2</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="22"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="19">
+        <f>((F1-1)*(F1-wzn)*(F1-wal))/((wsn-1)*(wsn-wzn)*(wsn-wal))</f>
+        <v>0.10066043625325014</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="19">
+        <f>((F1-1)*(F1-wsn)*(F1-wal))/((wzn-1)*(wzn-wsn)*(wzn-wal))</f>
+        <v>0.93228879936099973</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="19">
+        <f>((F1-1)*(F1-wsn)*(F1-wzn))/((wal-1)*(wal-wsn)*(wal-wzn))</f>
+        <v>-2.1984494284315294E-2</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <f>-0.00019948318</f>
+        <v>-1.9948318000000001E-4</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="50">
+        <v>-1.99515009237343E-4</v>
+      </c>
+      <c r="E9" s="23"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>-1.332309E-6</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="50">
+        <v>-1.2933998288050701E-6</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>-4.6999652999999998E-6</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="51">
+        <v>-4.7104297066317602E-6</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="33"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>3.3760086</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2.5689172999999998</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="46"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1.8927976799999999</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="47"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="33"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>3.37546422</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>2.56858298</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="38"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>1.89261521</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="39"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="41"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="41"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="41"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E24" s="39"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="41"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E25" s="42"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E20:J25"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C14:C16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
SPRT_Coeff_calc.py Wyznaczanie współczynników funkcji odchylenia z danych ze świadectwa
współczynniki PRT.sce Kalkulator Ze SciLaba
</commit_message>
<xml_diff>
--- a/Dane_termometrow.xlsx
+++ b/Dane_termometrow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="5685_1114" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
   <si>
     <t>Typ:</t>
   </si>
@@ -83,9 +83,6 @@
 k=2</t>
   </si>
   <si>
-    <t>961.78</t>
-  </si>
-  <si>
     <t>Wt</t>
   </si>
   <si>
@@ -236,7 +233,7 @@
     <numFmt numFmtId="166" formatCode="0.000000000"/>
     <numFmt numFmtId="167" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="168" formatCode="0.00000000E+00"/>
-    <numFmt numFmtId="176" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="169" formatCode="0.000000E+00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -533,6 +530,12 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -572,12 +575,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1219,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,33 +1234,33 @@
     <col min="8" max="8" width="13.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="F1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1274,10 +1271,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>3</v>
@@ -1289,12 +1286,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>4</v>
@@ -1306,7 +1303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>5686</v>
       </c>
@@ -1322,8 +1319,8 @@
       <c r="E4" s="4">
         <v>4.0999999999999997E-6</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>8</v>
+      <c r="F4" s="4">
+        <v>961.78</v>
       </c>
       <c r="G4" s="4">
         <v>4.2855629500000001</v>
@@ -1331,8 +1328,12 @@
       <c r="H4" s="4">
         <v>5.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f>F4-273.15</f>
+        <v>688.63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1346,7 +1347,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1360,7 +1361,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1374,7 +1375,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1382,7 +1383,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1390,18 +1391,18 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -1435,28 +1436,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="F1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1470,10 +1471,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>3</v>
@@ -1487,10 +1488,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>4</v>
@@ -1619,8 +1620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,7 +1633,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E1" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="26">
         <v>4.2855629500000001</v>
@@ -1640,7 +1641,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E2" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="25">
         <f>I5+I6*wrsn+I7*wrzn+I8*wral</f>
@@ -1649,7 +1650,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E3" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="25">
         <f>a*(F1-1)+b*(F1-1)^2+cc*(F1-1)^3</f>
@@ -1658,16 +1659,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E4" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="28">
         <f>F1-F2</f>
         <v>-8.1818808360178963E-4</v>
       </c>
-      <c r="H4" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="37"/>
+      <c r="H4" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="41"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="21"/>
@@ -1676,7 +1677,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="14"/>
       <c r="H5" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="19">
         <f>((F1-wsn)*(F1-wzn)*(F1-wal))/((1-wsn)*(1-wzn)*(1-wal))</f>
@@ -1692,7 +1693,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="14"/>
       <c r="H6" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" s="19">
         <f>((F1-1)*(F1-wzn)*(F1-wal))/((wsn-1)*(wsn-wzn)*(wsn-wal))</f>
@@ -1703,7 +1704,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="22"/>
@@ -1712,7 +1713,7 @@
       <c r="F7" s="21"/>
       <c r="G7" s="14"/>
       <c r="H7" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="19">
         <f>((F1-1)*(F1-wsn)*(F1-wal))/((wzn-1)*(wzn-wsn)*(wzn-wal))</f>
@@ -1726,13 +1727,13 @@
       <c r="B8" s="32"/>
       <c r="C8" s="22"/>
       <c r="D8" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="21"/>
       <c r="G8" s="14"/>
       <c r="H8" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" s="19">
         <f>((F1-1)*(F1-wsn)*(F1-wzn))/((wal-1)*(wal-wsn)*(wal-wzn))</f>
@@ -1746,10 +1747,10 @@
         <v>-2.6051786999999998E-4</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="22"/>
-      <c r="D9" s="51">
+      <c r="D9" s="38">
         <v>-2.1371537544641301E-4</v>
       </c>
       <c r="E9" s="23"/>
@@ -1765,10 +1766,10 @@
         <v>3.0380417000000001E-5</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="22"/>
-      <c r="D10" s="51">
+      <c r="D10" s="38">
         <v>-1.43251789292556E-5</v>
       </c>
       <c r="E10" s="22"/>
@@ -1782,9 +1783,9 @@
         <v>-9.4374361000000006E-6</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="52">
+        <v>32</v>
+      </c>
+      <c r="D11" s="39">
         <v>1.0884977044838E-6</v>
       </c>
       <c r="F11" s="16"/>
@@ -1793,21 +1794,21 @@
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="50">
+      <c r="A12" s="37">
         <f>((a*(A22-1)+b*(A22-1)^2+cc*(A22-1)^3)+A17-A22)/(-1*(A22-wal)^2)</f>
         <v>6.1990881333963544E-6</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="53">
+        <v>46</v>
+      </c>
+      <c r="D12" s="40">
         <f>((D9*(A22-1)+D10*(A22-1)^2+D11*(A22-1)^3)+A17-A22)/(-1*(A22-wal)^2)</f>
         <v>-4.7531160190024585E-5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="32"/>
     </row>
@@ -1816,10 +1817,10 @@
         <v>3.3760086</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>42</v>
+        <v>27</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1827,30 +1828,30 @@
         <v>2.5689172999999998</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="48"/>
+        <v>28</v>
+      </c>
+      <c r="C15" s="52"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>1.8927976799999999</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="49"/>
+        <v>29</v>
+      </c>
+      <c r="C16" s="53"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>4.28642053</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="32"/>
     </row>
@@ -1859,7 +1860,7 @@
         <v>3.3754346900000001</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1867,70 +1868,70 @@
         <v>2.5685510300000001</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="40"/>
+        <v>34</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>1.89259628</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="43"/>
+        <v>35</v>
+      </c>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="47"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>4.2855629500000001</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="43"/>
+        <v>43</v>
+      </c>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="47"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
       <c r="B23" s="34"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="43"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="47"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E24" s="41"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="43"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="47"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E25" s="44"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="46"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1948,7 +1949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1961,7 +1962,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E1" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="26">
         <v>2.5</v>
@@ -1969,7 +1970,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E2" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="25">
         <f>I5+I6*wrsn+I7*wrzn+I8*wral</f>
@@ -1978,7 +1979,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E3" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="25">
         <f>a*(F1-1)+b*(F1-1)^2+cc*(F1-1)^3</f>
@@ -1987,16 +1988,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E4" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="28">
         <f>F1-F2</f>
         <v>-3.1808238220687457E-4</v>
       </c>
-      <c r="H4" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="37"/>
+      <c r="H4" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="41"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="21"/>
@@ -2005,7 +2006,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="14"/>
       <c r="H5" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="19">
         <f>((F1-wsn)*(F1-wzn)*(F1-wal))/((1-wsn)*(1-wzn)*(1-wal))</f>
@@ -2021,7 +2022,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="14"/>
       <c r="H6" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" s="19">
         <f>((F1-1)*(F1-wzn)*(F1-wal))/((wsn-1)*(wsn-wzn)*(wsn-wal))</f>
@@ -2032,7 +2033,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="22"/>
@@ -2041,7 +2042,7 @@
       <c r="F7" s="21"/>
       <c r="G7" s="14"/>
       <c r="H7" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="19">
         <f>((F1-1)*(F1-wsn)*(F1-wal))/((wzn-1)*(wzn-wsn)*(wzn-wal))</f>
@@ -2055,13 +2056,13 @@
       <c r="B8" s="32"/>
       <c r="C8" s="22"/>
       <c r="D8" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="21"/>
       <c r="G8" s="14"/>
       <c r="H8" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" s="19">
         <f>((F1-1)*(F1-wsn)*(F1-wzn))/((wal-1)*(wal-wsn)*(wal-wzn))</f>
@@ -2076,7 +2077,7 @@
         <v>-1.9948318000000001E-4</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="35">
@@ -2095,7 +2096,7 @@
         <v>-1.332309E-6</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="35">
@@ -2112,7 +2113,7 @@
         <v>-4.6999652999999998E-6</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="36">
         <v>-4.7104297066317602E-6</v>
@@ -2128,7 +2129,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="32"/>
     </row>
@@ -2137,10 +2138,10 @@
         <v>3.3760086</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>42</v>
+        <v>27</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2148,18 +2149,18 @@
         <v>2.5689172999999998</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="48"/>
+        <v>28</v>
+      </c>
+      <c r="C15" s="52"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>1.8927976799999999</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="49"/>
+        <v>29</v>
+      </c>
+      <c r="C16" s="53"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
@@ -2167,7 +2168,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="32"/>
     </row>
@@ -2176,7 +2177,7 @@
         <v>3.37546422</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2184,66 +2185,66 @@
         <v>2.56858298</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="40"/>
+        <v>34</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>1.89261521</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="43"/>
+        <v>35</v>
+      </c>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="47"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
       <c r="B22" s="32"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="43"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="47"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
       <c r="B23" s="34"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="43"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="47"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E24" s="41"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="43"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="47"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E25" s="44"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="46"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>